<commit_message>
Update customer import spec
</commit_message>
<xml_diff>
--- a/spec/fixtures/invalid_customer_import.xlsx
+++ b/spec/fixtures/invalid_customer_import.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="3060" windowWidth="25120" windowHeight="17000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,6 @@
     <t>Billing State</t>
   </si>
   <si>
-    <t>Billing Zip Code</t>
-  </si>
-  <si>
     <t>Primary Shipping Street</t>
   </si>
   <si>
@@ -48,9 +45,6 @@
     <t>Primary Shipping State</t>
   </si>
   <si>
-    <t>Primary Shipping Zip Code</t>
-  </si>
-  <si>
     <t>Secondary Shipping Street</t>
   </si>
   <si>
@@ -60,9 +54,6 @@
     <t>Secondary Shipping State</t>
   </si>
   <si>
-    <t>Secondary Shipping Zip Code</t>
-  </si>
-  <si>
     <t>Bob</t>
   </si>
   <si>
@@ -112,6 +103,15 @@
   </si>
   <si>
     <t>Doe</t>
+  </si>
+  <si>
+    <t>Billing Zipcode</t>
+  </si>
+  <si>
+    <t>Primary Shipping Zipcode</t>
+  </si>
+  <si>
+    <t>Secondary Shipping Zipcode</t>
   </si>
 </sst>
 </file>
@@ -483,7 +483,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
@@ -504,72 +506,72 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
       <c r="N1" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F2">
         <v>27701</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J2">
         <v>27701</v>
       </c>
       <c r="K2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="M2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="N2">
         <v>27701</v>
@@ -577,43 +579,43 @@
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F3">
         <v>27702</v>
       </c>
       <c r="G3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J3">
         <v>27702</v>
       </c>
       <c r="K3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="M3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="N3">
         <v>27702</v>
@@ -621,31 +623,31 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F4">
         <v>27613</v>
       </c>
       <c r="G4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="I4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J4">
         <v>27613</v>
@@ -653,31 +655,31 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J5">
         <v>27701</v>
       </c>
       <c r="K5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="L5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="M5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="N5">
         <v>27701</v>

</xml_diff>